<commit_message>
import entities excel template fix
</commit_message>
<xml_diff>
--- a/src/assets/file/Import_Entities_Template.xlsx
+++ b/src/assets/file/Import_Entities_Template.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NestPublisher\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irfanul\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4BF48D-FACA-4CD9-BC17-111215EFDBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96127314-6895-4DBE-8E02-DFC4B1E2CC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2777270-ACCD-4CCF-837E-C188DD7609D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C78B644-D1B8-404E-BF5F-7D7A9502D109}"/>
   </bookViews>
   <sheets>
-    <sheet name="WTA" sheetId="1" r:id="rId1"/>
-    <sheet name="TPA" sheetId="2" r:id="rId2"/>
-    <sheet name="Treaty" sheetId="4" r:id="rId3"/>
+    <sheet name="ImportEntitiesTemplate" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,46 +25,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>BriefType</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>ShortStory</t>
-  </si>
-  <si>
-    <t>LongStory</t>
-  </si>
-  <si>
-    <t>CountryCode</t>
-  </si>
-  <si>
-    <t>RegFollowerLink</t>
-  </si>
-  <si>
-    <t>WtaBriefing</t>
-  </si>
-  <si>
-    <t>TpaBriefing</t>
-  </si>
-  <si>
-    <t>TreatyBriefing</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Entity Name</t>
+  </si>
+  <si>
+    <t>Incorporation Jurisdiction</t>
+  </si>
+  <si>
+    <t>Sub National</t>
+  </si>
+  <si>
+    <t>Tax Residence</t>
+  </si>
+  <si>
+    <t>Business Type</t>
+  </si>
+  <si>
+    <t>Business SIC Code</t>
+  </si>
+  <si>
+    <t>Ownership</t>
+  </si>
+  <si>
+    <t>Ownership %</t>
+  </si>
+  <si>
+    <t>Tax Characterization</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,27 +72,26 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -105,27 +99,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,26 +439,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE9AC60-9D60-4CC3-A414-7E58CA8902C1}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02B3CE2-0EA3-4696-8CCF-85C3FD38BFFF}">
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" customWidth="1"/>
-    <col min="7" max="7" width="60.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -468,149 +471,25 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D29998C-3F8D-41BE-8532-3AE3F84B63CB}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.5703125" customWidth="1"/>
-    <col min="6" max="6" width="62" customWidth="1"/>
-    <col min="7" max="7" width="42.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4314AB0-CBA0-458D-A8CA-7FC92FFC1A1F}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" customWidth="1"/>
-    <col min="7" max="7" width="68.85546875" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>